<commit_message>
Son test çalışır hale geldi.
</commit_message>
<xml_diff>
--- a/mangala-senaryo.xlsx
+++ b/mangala-senaryo.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,27 +20,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="11">
   <si>
     <t xml:space="preserve">1-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-2</t>
   </si>
   <si>
     <t xml:space="preserve">1-5</t>
   </si>
   <si>
+    <t xml:space="preserve">2-2</t>
+  </si>
+  <si>
     <t xml:space="preserve">2-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3</t>
   </si>
   <si>
     <t xml:space="preserve">1-4</t>
   </si>
   <si>
-    <t xml:space="preserve">2-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2-2</t>
+    <t xml:space="preserve">1-1</t>
   </si>
   <si>
     <t xml:space="preserve">2-4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-0</t>
   </si>
 </sst>
 </file>
@@ -55,6 +67,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -140,12 +153,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -155,16 +168,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W71"/>
+  <dimension ref="A1:AJ120"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q71" activeCellId="0" sqref="Q71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q109" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AI115" activeCellId="0" sqref="AI115"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="23" min="1" style="0" width="5.20408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="0" width="11.5204081632653"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="1" style="0" width="5.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="25" style="0" width="5.2"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -184,6 +197,14 @@
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
+      <c r="AA1" s="1"/>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
+      <c r="AE1" s="1"/>
+      <c r="AF1" s="1"/>
+      <c r="AG1" s="1"/>
+      <c r="AH1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="1"/>
@@ -202,6 +223,14 @@
       <c r="U2" s="1"/>
       <c r="V2" s="1"/>
       <c r="W2" s="1"/>
+      <c r="AA2" s="1"/>
+      <c r="AB2" s="1"/>
+      <c r="AC2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
+      <c r="AF2" s="1"/>
+      <c r="AG2" s="1"/>
+      <c r="AH2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="1" t="n">
@@ -248,9 +277,31 @@
         <v>0</v>
       </c>
       <c r="W3" s="1"/>
+      <c r="AA3" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB3" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC3" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD3" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE3" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="3"/>
@@ -273,7 +324,7 @@
         <v>4</v>
       </c>
       <c r="J4" s="3"/>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="1" t="n">
         <v>1</v>
       </c>
       <c r="P4" s="3"/>
@@ -296,8 +347,36 @@
         <v>4</v>
       </c>
       <c r="W4" s="3"/>
+      <c r="Y4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC4" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD4" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE4" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF4" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG4" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH4" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="n">
         <v>4</v>
@@ -318,6 +397,7 @@
         <v>4</v>
       </c>
       <c r="J5" s="3"/>
+      <c r="N5" s="1"/>
       <c r="P5" s="3"/>
       <c r="Q5" s="3" t="n">
         <v>4</v>
@@ -338,6 +418,27 @@
         <v>4</v>
       </c>
       <c r="W5" s="3"/>
+      <c r="Y5" s="1"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG5" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="0" t="n">
@@ -382,6 +483,27 @@
       <c r="W6" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="AB6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF6" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH6" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="n">
@@ -426,9 +548,30 @@
       <c r="V9" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="AA9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB9" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC9" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD9" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE9" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG9" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="3"/>
@@ -453,7 +596,7 @@
       <c r="J10" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="N10" s="0" t="s">
+      <c r="N10" s="1" t="s">
         <v>0</v>
       </c>
       <c r="P10" s="3"/>
@@ -478,8 +621,36 @@
       <c r="W10" s="3" t="n">
         <v>1</v>
       </c>
+      <c r="Y10" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA10" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG10" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH10" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="n">
         <v>4</v>
@@ -500,6 +671,7 @@
         <v>5</v>
       </c>
       <c r="J11" s="3"/>
+      <c r="N11" s="1"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3" t="n">
         <v>4</v>
@@ -520,6 +692,27 @@
         <v>5</v>
       </c>
       <c r="W11" s="3"/>
+      <c r="Y11" s="1"/>
+      <c r="AA11" s="3"/>
+      <c r="AB11" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC11" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD11" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE11" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF11" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG11" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH11" s="3"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="2" t="n">
@@ -562,6 +755,27 @@
         <v>5</v>
       </c>
       <c r="W12" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD12" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE12" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF12" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG12" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH12" s="0" t="n">
         <v>6</v>
       </c>
     </row>
@@ -578,6 +792,12 @@
       <c r="T13" s="2"/>
       <c r="U13" s="2"/>
       <c r="V13" s="2"/>
+      <c r="AB13" s="2"/>
+      <c r="AC13" s="2"/>
+      <c r="AD13" s="2"/>
+      <c r="AE13" s="2"/>
+      <c r="AF13" s="2"/>
+      <c r="AG13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D14" s="2"/>
@@ -592,6 +812,12 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2"/>
+      <c r="AB14" s="2"/>
+      <c r="AC14" s="2"/>
+      <c r="AD14" s="2"/>
+      <c r="AE14" s="2"/>
+      <c r="AF14" s="2"/>
+      <c r="AG14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C15" s="0" t="n">
@@ -636,10 +862,31 @@
       <c r="V15" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="AA15" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB15" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC15" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD15" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE15" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG15" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>1</v>
+      <c r="A16" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3" t="n">
@@ -663,8 +910,8 @@
       <c r="J16" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="N16" s="0" t="s">
-        <v>1</v>
+      <c r="N16" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="P16" s="3"/>
       <c r="Q16" s="3" t="n">
@@ -688,8 +935,36 @@
       <c r="W16" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="Y16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA16" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC16" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD16" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE16" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF16" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG16" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AH16" s="3" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="n">
         <v>4</v>
@@ -710,6 +985,7 @@
         <v>1</v>
       </c>
       <c r="J17" s="3"/>
+      <c r="N17" s="1"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3" t="n">
         <v>4</v>
@@ -730,6 +1006,27 @@
         <v>1</v>
       </c>
       <c r="W17" s="3"/>
+      <c r="Y17" s="1"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC17" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD17" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE17" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF17" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG17" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH17" s="3"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="2" t="n">
@@ -772,6 +1069,27 @@
         <v>5</v>
       </c>
       <c r="W18" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD18" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE18" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF18" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG18" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH18" s="0" t="n">
         <v>6</v>
       </c>
     </row>
@@ -788,6 +1106,12 @@
       <c r="T19" s="2"/>
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
+      <c r="AB19" s="2"/>
+      <c r="AC19" s="2"/>
+      <c r="AD19" s="2"/>
+      <c r="AE19" s="2"/>
+      <c r="AF19" s="2"/>
+      <c r="AG19" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="n">
@@ -832,10 +1156,31 @@
       <c r="V21" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="AA21" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB21" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC21" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD21" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE21" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF21" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG21" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>2</v>
+      <c r="A22" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>1</v>
@@ -861,8 +1206,8 @@
       <c r="J22" s="3" t="n">
         <v>2</v>
       </c>
-      <c r="N22" s="0" t="s">
-        <v>2</v>
+      <c r="N22" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="P22" s="3" t="n">
         <v>1</v>
@@ -888,8 +1233,36 @@
       <c r="W22" s="3" t="n">
         <v>2</v>
       </c>
+      <c r="Y22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC22" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD22" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE22" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF22" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG22" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH22" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1"/>
       <c r="C23" s="3"/>
       <c r="D23" s="3" t="n">
         <v>5</v>
@@ -910,6 +1283,7 @@
         <v>1</v>
       </c>
       <c r="J23" s="3"/>
+      <c r="N23" s="1"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3" t="n">
         <v>5</v>
@@ -930,6 +1304,27 @@
         <v>1</v>
       </c>
       <c r="W23" s="3"/>
+      <c r="Y23" s="1"/>
+      <c r="AA23" s="3"/>
+      <c r="AB23" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC23" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD23" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE23" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF23" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG23" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D24" s="2" t="n">
@@ -974,6 +1369,27 @@
       <c r="W24" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="AB24" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD24" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE24" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF24" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG24" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH24" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C27" s="0" t="n">
@@ -1018,10 +1434,31 @@
       <c r="V27" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="AA27" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB27" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC27" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD27" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE27" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF27" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG27" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>1</v>
+      <c r="A28" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="C28" s="3" t="n">
         <v>1</v>
@@ -1047,8 +1484,8 @@
       <c r="J28" s="3" t="n">
         <v>3</v>
       </c>
-      <c r="N28" s="0" t="s">
-        <v>1</v>
+      <c r="N28" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="P28" s="3" t="n">
         <v>1</v>
@@ -1074,8 +1511,36 @@
       <c r="W28" s="3" t="n">
         <v>3</v>
       </c>
+      <c r="Y28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA28" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB28" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC28" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD28" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE28" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF28" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG28" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH28" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="n">
         <v>5</v>
@@ -1096,6 +1561,7 @@
         <v>0</v>
       </c>
       <c r="J29" s="3"/>
+      <c r="N29" s="1"/>
       <c r="P29" s="3"/>
       <c r="Q29" s="3" t="n">
         <v>5</v>
@@ -1116,6 +1582,27 @@
         <v>0</v>
       </c>
       <c r="W29" s="3"/>
+      <c r="Y29" s="1"/>
+      <c r="AA29" s="3"/>
+      <c r="AB29" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC29" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD29" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE29" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF29" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AG29" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D30" s="2" t="n">
@@ -1160,6 +1647,27 @@
       <c r="W30" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="AB30" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD30" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE30" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF30" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG30" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH30" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C33" s="0" t="n">
@@ -1204,10 +1712,31 @@
       <c r="V33" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="AA33" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB33" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC33" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD33" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE33" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF33" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG33" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>3</v>
+      <c r="A34" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C34" s="3" t="n">
         <v>1</v>
@@ -1233,8 +1762,8 @@
       <c r="J34" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="N34" s="0" t="s">
-        <v>3</v>
+      <c r="N34" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="P34" s="3" t="n">
         <v>1</v>
@@ -1260,8 +1789,36 @@
       <c r="W34" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="Y34" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB34" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC34" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE34" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF34" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG34" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH34" s="3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="n">
         <v>5</v>
@@ -1282,6 +1839,7 @@
         <v>1</v>
       </c>
       <c r="J35" s="3"/>
+      <c r="N35" s="1"/>
       <c r="P35" s="3"/>
       <c r="Q35" s="3" t="n">
         <v>5</v>
@@ -1302,6 +1860,27 @@
         <v>1</v>
       </c>
       <c r="W35" s="3"/>
+      <c r="Y35" s="1"/>
+      <c r="AA35" s="3"/>
+      <c r="AB35" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC35" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD35" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE35" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF35" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AG35" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D36" s="2" t="n">
@@ -1346,6 +1925,27 @@
       <c r="W36" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="AB36" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD36" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE36" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF36" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG36" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH36" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C39" s="0" t="n">
@@ -1390,10 +1990,31 @@
       <c r="V39" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="AA39" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB39" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC39" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD39" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE39" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF39" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG39" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="0" t="s">
-        <v>2</v>
+      <c r="A40" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C40" s="3" t="n">
         <v>2</v>
@@ -1419,8 +2040,8 @@
       <c r="J40" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="N40" s="0" t="s">
-        <v>2</v>
+      <c r="N40" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="P40" s="3" t="n">
         <v>2</v>
@@ -1446,8 +2067,40 @@
       <c r="W40" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="Y40" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA40" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB40" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC40" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD40" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AE40" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF40" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG40" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH40" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ40" s="0" t="n">
+        <f aca="false">AA40+AB40+AC40+AD40+AE40+AF40+AG40+AH40+AG41+AF41+AE41+AD41+AC41+AB41</f>
+        <v>48</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="n">
         <v>5</v>
@@ -1468,6 +2121,7 @@
         <v>1</v>
       </c>
       <c r="J41" s="3"/>
+      <c r="N41" s="1"/>
       <c r="P41" s="3"/>
       <c r="Q41" s="3" t="n">
         <v>5</v>
@@ -1488,6 +2142,27 @@
         <v>1</v>
       </c>
       <c r="W41" s="3"/>
+      <c r="Y41" s="1"/>
+      <c r="AA41" s="3"/>
+      <c r="AB41" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC41" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD41" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE41" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF41" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AG41" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D42" s="2" t="n">
@@ -1532,6 +2207,27 @@
       <c r="W42" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="AB42" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD42" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE42" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF42" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG42" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH42" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C45" s="0" t="n">
@@ -1576,10 +2272,31 @@
       <c r="V45" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="AA45" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB45" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC45" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD45" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE45" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF45" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG45" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="s">
-        <v>4</v>
+      <c r="A46" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C46" s="3" t="n">
         <v>3</v>
@@ -1605,8 +2322,8 @@
       <c r="J46" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="N46" s="0" t="s">
-        <v>4</v>
+      <c r="N46" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="P46" s="3" t="n">
         <v>3</v>
@@ -1632,8 +2349,36 @@
       <c r="W46" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="Y46" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA46" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB46" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC46" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD46" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE46" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF46" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG46" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH46" s="3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="n">
         <v>5</v>
@@ -1654,6 +2399,7 @@
         <v>1</v>
       </c>
       <c r="J47" s="3"/>
+      <c r="N47" s="1"/>
       <c r="P47" s="3"/>
       <c r="Q47" s="3" t="n">
         <v>5</v>
@@ -1674,6 +2420,27 @@
         <v>1</v>
       </c>
       <c r="W47" s="3"/>
+      <c r="Y47" s="1"/>
+      <c r="AA47" s="3"/>
+      <c r="AB47" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC47" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD47" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE47" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF47" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG47" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AH47" s="3"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D48" s="2" t="n">
@@ -1718,6 +2485,27 @@
       <c r="W48" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="AB48" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC48" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD48" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE48" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF48" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG48" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH48" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="0" t="n">
@@ -1762,10 +2550,31 @@
       <c r="V51" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="AA51" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB51" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC51" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD51" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE51" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF51" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG51" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="s">
-        <v>2</v>
+      <c r="A52" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="C52" s="3" t="n">
         <v>4</v>
@@ -1791,8 +2600,8 @@
       <c r="J52" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="N52" s="0" t="s">
-        <v>2</v>
+      <c r="N52" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="P52" s="3" t="n">
         <v>4</v>
@@ -1818,8 +2627,36 @@
       <c r="W52" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="Y52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA52" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB52" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC52" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD52" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE52" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF52" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG52" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH52" s="3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1"/>
       <c r="C53" s="3"/>
       <c r="D53" s="3" t="n">
         <v>5</v>
@@ -1840,6 +2677,7 @@
         <v>1</v>
       </c>
       <c r="J53" s="3"/>
+      <c r="N53" s="1"/>
       <c r="P53" s="3"/>
       <c r="Q53" s="3" t="n">
         <v>5</v>
@@ -1860,6 +2698,27 @@
         <v>1</v>
       </c>
       <c r="W53" s="3"/>
+      <c r="Y53" s="1"/>
+      <c r="AA53" s="3"/>
+      <c r="AB53" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC53" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD53" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE53" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF53" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG53" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AH53" s="3"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D54" s="2" t="n">
@@ -1904,6 +2763,27 @@
       <c r="W54" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="AB54" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC54" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD54" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE54" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF54" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG54" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH54" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C57" s="0" t="n">
@@ -1948,10 +2828,31 @@
       <c r="V57" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="AA57" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB57" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC57" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD57" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE57" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF57" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG57" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="s">
-        <v>5</v>
+      <c r="A58" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="C58" s="3" t="n">
         <v>5</v>
@@ -1977,8 +2878,8 @@
       <c r="J58" s="3" t="n">
         <v>10</v>
       </c>
-      <c r="N58" s="0" t="s">
-        <v>6</v>
+      <c r="N58" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="P58" s="3" t="n">
         <v>11</v>
@@ -2004,8 +2905,36 @@
       <c r="W58" s="3" t="n">
         <v>10</v>
       </c>
+      <c r="Y58" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA58" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB58" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC58" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD58" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE58" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF58" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG58" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH58" s="3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="n">
         <v>5</v>
@@ -2026,6 +2955,7 @@
         <v>1</v>
       </c>
       <c r="J59" s="3"/>
+      <c r="N59" s="1"/>
       <c r="P59" s="3"/>
       <c r="Q59" s="3" t="n">
         <v>6</v>
@@ -2046,6 +2976,27 @@
         <v>1</v>
       </c>
       <c r="W59" s="3"/>
+      <c r="Y59" s="1"/>
+      <c r="AA59" s="3"/>
+      <c r="AB59" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC59" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD59" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE59" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF59" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG59" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AH59" s="3"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D60" s="2" t="n">
@@ -2090,6 +3041,27 @@
       <c r="W60" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="AB60" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC60" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD60" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE60" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF60" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG60" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH60" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P63" s="0" t="n">
@@ -2113,10 +3085,31 @@
       <c r="V63" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="AA63" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB63" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC63" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD63" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE63" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF63" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG63" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N64" s="0" t="s">
-        <v>1</v>
+      <c r="N64" s="1" t="s">
+        <v>2</v>
       </c>
       <c r="P64" s="3" t="n">
         <v>11</v>
@@ -2142,8 +3135,36 @@
       <c r="W64" s="3" t="n">
         <v>11</v>
       </c>
+      <c r="Y64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA64" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB64" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC64" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD64" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE64" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF64" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG64" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH64" s="3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N65" s="1"/>
       <c r="P65" s="3"/>
       <c r="Q65" s="3" t="n">
         <v>6</v>
@@ -2164,6 +3185,27 @@
         <v>0</v>
       </c>
       <c r="W65" s="3"/>
+      <c r="Y65" s="1"/>
+      <c r="AA65" s="3"/>
+      <c r="AB65" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC65" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD65" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE65" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF65" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG65" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AH65" s="3"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q66" s="2" t="n">
@@ -2187,6 +3229,27 @@
       <c r="W66" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="AB66" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC66" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD66" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE66" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF66" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG66" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH66" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P68" s="0" t="n">
@@ -2212,8 +3275,8 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="N69" s="0" t="s">
-        <v>3</v>
+      <c r="N69" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="P69" s="3" t="n">
         <v>11</v>
@@ -2239,8 +3302,30 @@
       <c r="W69" s="3" t="n">
         <v>18</v>
       </c>
+      <c r="AA69" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB69" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC69" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD69" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE69" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF69" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG69" s="2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N70" s="1"/>
       <c r="P70" s="3"/>
       <c r="Q70" s="3" t="n">
         <v>6</v>
@@ -2261,6 +3346,33 @@
         <v>0</v>
       </c>
       <c r="W70" s="3"/>
+      <c r="Y70" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA70" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB70" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC70" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD70" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE70" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF70" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG70" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH70" s="3" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="Q71" s="2" t="n">
@@ -2284,79 +3396,967 @@
       <c r="W71" s="0" t="n">
         <v>6</v>
       </c>
+      <c r="Y71" s="1"/>
+      <c r="AA71" s="3"/>
+      <c r="AB71" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC71" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD71" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE71" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF71" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG71" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AH71" s="3"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB72" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC72" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD72" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE72" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF72" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG72" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH72" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA75" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB75" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC75" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD75" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE75" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF75" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG75" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA76" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB76" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC76" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD76" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE76" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF76" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG76" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH76" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y77" s="1"/>
+      <c r="AA77" s="3"/>
+      <c r="AB77" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC77" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD77" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE77" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF77" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG77" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AH77" s="3"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB78" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC78" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD78" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE78" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF78" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG78" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH78" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA81" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB81" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC81" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD81" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE81" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF81" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG81" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y82" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA82" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB82" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC82" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD82" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE82" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF82" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AG82" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH82" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y83" s="1"/>
+      <c r="AA83" s="3"/>
+      <c r="AB83" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC83" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD83" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE83" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF83" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG83" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH83" s="3"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB84" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC84" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD84" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE84" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF84" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG84" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH84" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA87" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB87" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC87" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD87" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE87" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF87" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG87" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y88" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA88" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB88" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC88" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD88" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE88" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF88" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG88" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH88" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y89" s="1"/>
+      <c r="AA89" s="3"/>
+      <c r="AB89" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC89" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD89" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE89" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF89" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG89" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH89" s="3"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB90" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC90" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD90" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE90" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF90" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG90" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH90" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA93" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB93" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC93" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD93" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE93" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF93" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG93" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y94" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA94" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB94" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC94" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD94" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE94" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF94" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG94" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH94" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y95" s="1"/>
+      <c r="AA95" s="3"/>
+      <c r="AB95" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC95" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD95" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE95" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF95" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG95" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH95" s="3"/>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB96" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC96" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD96" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE96" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF96" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG96" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH96" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA99" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB99" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC99" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD99" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE99" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF99" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG99" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y100" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA100" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB100" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC100" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD100" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE100" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF100" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG100" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH100" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y101" s="1"/>
+      <c r="AA101" s="3"/>
+      <c r="AB101" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC101" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD101" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE101" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF101" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG101" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH101" s="3"/>
+    </row>
+    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB102" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC102" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD102" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE102" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF102" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG102" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH102" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA105" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB105" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC105" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD105" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE105" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF105" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG105" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y106" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA106" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB106" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC106" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD106" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE106" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF106" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG106" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH106" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y107" s="1"/>
+      <c r="AA107" s="3"/>
+      <c r="AB107" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC107" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD107" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE107" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF107" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG107" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH107" s="3"/>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB108" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC108" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD108" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE108" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF108" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG108" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH108" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA111" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB111" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC111" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD111" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE111" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF111" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG111" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y112" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AA112" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB112" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC112" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD112" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE112" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF112" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG112" s="3" t="n">
+        <v>6</v>
+      </c>
+      <c r="AH112" s="3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y113" s="1"/>
+      <c r="AA113" s="3"/>
+      <c r="AB113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC113" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD113" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE113" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF113" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG113" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="AH113" s="3"/>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB114" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC114" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD114" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE114" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF114" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG114" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH114" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA117" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="AB117" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC117" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AD117" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AE117" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AF117" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG117" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y118" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA118" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AB118" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC118" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AD118" s="3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AE118" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF118" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG118" s="3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AH118" s="3" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y119" s="1"/>
+      <c r="AA119" s="3"/>
+      <c r="AB119" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC119" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="AD119" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE119" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="AF119" s="3" t="n">
+        <v>2</v>
+      </c>
+      <c r="AG119" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH119" s="3"/>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AB120" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC120" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD120" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE120" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="AF120" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="AG120" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AH120" s="0" t="n">
+        <v>6</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="66">
+  <mergeCells count="126">
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="C4:C5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="N4:N5"/>
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="W4:W5"/>
+    <mergeCell ref="Y4:Y5"/>
+    <mergeCell ref="AA4:AA5"/>
+    <mergeCell ref="AH4:AH5"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="J10:J11"/>
     <mergeCell ref="N10:N11"/>
     <mergeCell ref="P10:P11"/>
     <mergeCell ref="W10:W11"/>
+    <mergeCell ref="Y10:Y11"/>
+    <mergeCell ref="AA10:AA11"/>
+    <mergeCell ref="AH10:AH11"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="C16:C17"/>
     <mergeCell ref="J16:J17"/>
     <mergeCell ref="N16:N17"/>
     <mergeCell ref="P16:P17"/>
     <mergeCell ref="W16:W17"/>
+    <mergeCell ref="Y16:Y17"/>
+    <mergeCell ref="AA16:AA17"/>
+    <mergeCell ref="AH16:AH17"/>
     <mergeCell ref="A22:A23"/>
     <mergeCell ref="C22:C23"/>
     <mergeCell ref="J22:J23"/>
     <mergeCell ref="N22:N23"/>
     <mergeCell ref="P22:P23"/>
     <mergeCell ref="W22:W23"/>
+    <mergeCell ref="Y22:Y23"/>
+    <mergeCell ref="AA22:AA23"/>
+    <mergeCell ref="AH22:AH23"/>
     <mergeCell ref="A28:A29"/>
     <mergeCell ref="C28:C29"/>
     <mergeCell ref="J28:J29"/>
     <mergeCell ref="N28:N29"/>
     <mergeCell ref="P28:P29"/>
     <mergeCell ref="W28:W29"/>
+    <mergeCell ref="Y28:Y29"/>
+    <mergeCell ref="AA28:AA29"/>
+    <mergeCell ref="AH28:AH29"/>
     <mergeCell ref="A34:A35"/>
     <mergeCell ref="C34:C35"/>
     <mergeCell ref="J34:J35"/>
     <mergeCell ref="N34:N35"/>
     <mergeCell ref="P34:P35"/>
     <mergeCell ref="W34:W35"/>
+    <mergeCell ref="Y34:Y35"/>
+    <mergeCell ref="AA34:AA35"/>
+    <mergeCell ref="AH34:AH35"/>
     <mergeCell ref="A40:A41"/>
     <mergeCell ref="C40:C41"/>
     <mergeCell ref="J40:J41"/>
     <mergeCell ref="N40:N41"/>
     <mergeCell ref="P40:P41"/>
     <mergeCell ref="W40:W41"/>
+    <mergeCell ref="Y40:Y41"/>
+    <mergeCell ref="AA40:AA41"/>
+    <mergeCell ref="AH40:AH41"/>
     <mergeCell ref="A46:A47"/>
     <mergeCell ref="C46:C47"/>
     <mergeCell ref="J46:J47"/>
     <mergeCell ref="N46:N47"/>
     <mergeCell ref="P46:P47"/>
     <mergeCell ref="W46:W47"/>
+    <mergeCell ref="Y46:Y47"/>
+    <mergeCell ref="AA46:AA47"/>
+    <mergeCell ref="AH46:AH47"/>
     <mergeCell ref="A52:A53"/>
     <mergeCell ref="C52:C53"/>
     <mergeCell ref="J52:J53"/>
     <mergeCell ref="N52:N53"/>
     <mergeCell ref="P52:P53"/>
     <mergeCell ref="W52:W53"/>
+    <mergeCell ref="Y52:Y53"/>
+    <mergeCell ref="AA52:AA53"/>
+    <mergeCell ref="AH52:AH53"/>
     <mergeCell ref="A58:A59"/>
     <mergeCell ref="C58:C59"/>
     <mergeCell ref="J58:J59"/>
     <mergeCell ref="N58:N59"/>
     <mergeCell ref="P58:P59"/>
     <mergeCell ref="W58:W59"/>
+    <mergeCell ref="Y58:Y59"/>
+    <mergeCell ref="AA58:AA59"/>
+    <mergeCell ref="AH58:AH59"/>
     <mergeCell ref="N64:N65"/>
     <mergeCell ref="P64:P65"/>
     <mergeCell ref="W64:W65"/>
+    <mergeCell ref="Y64:Y65"/>
+    <mergeCell ref="AA64:AA65"/>
+    <mergeCell ref="AH64:AH65"/>
     <mergeCell ref="N69:N70"/>
     <mergeCell ref="P69:P70"/>
     <mergeCell ref="W69:W70"/>
+    <mergeCell ref="Y70:Y71"/>
+    <mergeCell ref="AA70:AA71"/>
+    <mergeCell ref="AH70:AH71"/>
+    <mergeCell ref="Y76:Y77"/>
+    <mergeCell ref="AA76:AA77"/>
+    <mergeCell ref="AH76:AH77"/>
+    <mergeCell ref="Y82:Y83"/>
+    <mergeCell ref="AA82:AA83"/>
+    <mergeCell ref="AH82:AH83"/>
+    <mergeCell ref="Y88:Y89"/>
+    <mergeCell ref="AA88:AA89"/>
+    <mergeCell ref="AH88:AH89"/>
+    <mergeCell ref="Y94:Y95"/>
+    <mergeCell ref="AA94:AA95"/>
+    <mergeCell ref="AH94:AH95"/>
+    <mergeCell ref="Y100:Y101"/>
+    <mergeCell ref="AA100:AA101"/>
+    <mergeCell ref="AH100:AH101"/>
+    <mergeCell ref="Y106:Y107"/>
+    <mergeCell ref="AA106:AA107"/>
+    <mergeCell ref="AH106:AH107"/>
+    <mergeCell ref="Y112:Y113"/>
+    <mergeCell ref="AA112:AA113"/>
+    <mergeCell ref="AH112:AH113"/>
+    <mergeCell ref="Y118:Y119"/>
+    <mergeCell ref="AA118:AA119"/>
+    <mergeCell ref="AH118:AH119"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>

</xml_diff>